<commit_message>
adding tests to masterControllerSpec.js and updating doc
</commit_message>
<xml_diff>
--- a/JasmineCheatSheet.xlsx
+++ b/JasmineCheatSheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>Beginning steps:</t>
   </si>
@@ -115,9 +115,6 @@
     </r>
   </si>
   <si>
-    <t>compare against expected values</t>
-  </si>
-  <si>
     <t>skip test ( note the x )</t>
   </si>
   <si>
@@ -175,6 +172,12 @@
     <t>toBe</t>
   </si>
   <si>
+    <t>toEqual</t>
+  </si>
+  <si>
+    <t>toMatch</t>
+  </si>
+  <si>
     <r>
       <t>expect</t>
     </r>
@@ -185,6 +188,118 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
+      <t>(msg).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6F42C1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>toMatch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF032F62"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/abc/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>toBeDefined</t>
+  </si>
+  <si>
+    <t>toBeUndefined</t>
+  </si>
+  <si>
+    <t>toBeTruthy</t>
+  </si>
+  <si>
+    <r>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF032F62"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'a'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6F42C1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>toBeTruthy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>();</t>
+    </r>
+  </si>
+  <si>
+    <t>toBeFalsy</t>
+  </si>
+  <si>
+    <r>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
       <t>(obj).</t>
     </r>
     <r>
@@ -194,7 +309,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>toBe</t>
+      <t>toBeFalsy</t>
     </r>
     <r>
       <rPr>
@@ -203,6 +318,58 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
+      <t>();</t>
+    </r>
+  </si>
+  <si>
+    <t>toContain</t>
+  </si>
+  <si>
+    <r>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(arr).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6F42C1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>toContain</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>();</t>
+    </r>
+  </si>
+  <si>
+    <t>toBeLessThan</t>
+  </si>
+  <si>
+    <r>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
       <t>(</t>
     </r>
     <r>
@@ -212,7 +379,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>null</t>
+      <t>21</t>
     </r>
     <r>
       <rPr>
@@ -221,8 +388,61 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6F42C1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>toBeLessThan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF005CC5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>42</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
       <t>);</t>
     </r>
+  </si>
+  <si>
+    <t>toBeGreaterThan</t>
+  </si>
+  <si>
+    <r>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
     <r>
       <rPr>
         <sz val="10"/>
@@ -230,11 +450,56 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>M</t>
-    </r>
-  </si>
-  <si>
-    <t>toEqual</t>
+      <t>42</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6F42C1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>toBeGreaterThan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF005CC5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>toBeCloseTo</t>
   </si>
   <si>
     <r>
@@ -247,6 +512,130 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF005CC5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6F42C1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>toBeCloseTo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF005CC5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1.23</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF005CC5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>toThrow</t>
+  </si>
+  <si>
+    <r>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(fnct).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6F42C1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>toThrow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>();</t>
+    </r>
+  </si>
+  <si>
+    <t>toThrowError</t>
+  </si>
+  <si>
+    <r>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
       <t>(obj).</t>
     </r>
     <r>
@@ -256,7 +645,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>toEqual</t>
+      <t>toThrowError</t>
     </r>
     <r>
       <rPr>
@@ -265,626 +654,11 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>({id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFD73A49"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF005CC5"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>});</t>
-    </r>
-  </si>
-  <si>
-    <t>toMatch</t>
-  </si>
-  <si>
-    <r>
-      <t>expect</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(msg).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6F42C1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>toMatch</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF032F62"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>/abc/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>);</t>
-    </r>
-  </si>
-  <si>
-    <t>toBeDefined</t>
-  </si>
-  <si>
-    <r>
-      <t>expect</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(obj).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6F42C1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>toBeDefined</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
       <t>();</t>
     </r>
   </si>
   <si>
-    <t>toBeUndefined</t>
-  </si>
-  <si>
-    <r>
-      <t>expect</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(obj).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6F42C1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>toBeUndefined</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>();</t>
-    </r>
-  </si>
-  <si>
-    <t>toBeTruthy</t>
-  </si>
-  <si>
-    <r>
-      <t>expect</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF032F62"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>'a'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6F42C1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>toBeTruthy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>();</t>
-    </r>
-  </si>
-  <si>
-    <t>toBeFalsy</t>
-  </si>
-  <si>
-    <r>
-      <t>expect</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(obj).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6F42C1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>toBeFalsy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>();</t>
-    </r>
-  </si>
-  <si>
-    <t>toContain</t>
-  </si>
-  <si>
-    <r>
-      <t>expect</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(arr).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6F42C1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>toContain</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>();</t>
-    </r>
-  </si>
-  <si>
-    <t>toBeLessThan</t>
-  </si>
-  <si>
-    <r>
-      <t>expect</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF005CC5"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>21</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6F42C1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>toBeLessThan</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF005CC5"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>42</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>);</t>
-    </r>
-  </si>
-  <si>
-    <t>toBeGreaterThan</t>
-  </si>
-  <si>
-    <r>
-      <t>expect</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF005CC5"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>42</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6F42C1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>toBeGreaterThan</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF005CC5"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>21</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>);</t>
-    </r>
-  </si>
-  <si>
-    <t>toBeCloseTo</t>
-  </si>
-  <si>
-    <r>
-      <t>expect</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF005CC5"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>1.2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6F42C1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>toBeCloseTo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF005CC5"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>1.23</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF005CC5"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>);</t>
-    </r>
-  </si>
-  <si>
-    <t>toThrow</t>
-  </si>
-  <si>
-    <r>
-      <t>expect</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(fnct).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6F42C1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>toThrow</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>();</t>
-    </r>
-  </si>
-  <si>
-    <t>toThrowError</t>
-  </si>
-  <si>
-    <r>
-      <t>expect</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(obj).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6F42C1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>toThrowError</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>();</t>
-    </r>
-  </si>
-  <si>
     <t>toBeNull</t>
-  </si>
-  <si>
-    <r>
-      <t>expect</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(obj).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6F42C1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>toBeNull</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>();</t>
-    </r>
   </si>
   <si>
     <t>not</t>
@@ -1480,14 +1254,590 @@
     <t>individual test/spec</t>
   </si>
   <si>
-    <t>suite of tests/specs</t>
+    <t>importing alias</t>
+  </si>
+  <si>
+    <t>alias</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$rootScope is the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>constructor variable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">controller service from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Angular</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">eventNames is the other </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>constructor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> param we need</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$rootScope is a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>constructor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> param we need </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MasterController is the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>class,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> need its params</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">angular </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>mock module</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>angular</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> injector service</t>
+    </r>
+  </si>
+  <si>
+    <t>instantiate controller</t>
+  </si>
+  <si>
+    <t>instantiating sut</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">beforeEach( () =&gt; ) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>run prior to each it in the describe</t>
+    </r>
+  </si>
+  <si>
+    <t>compare against expected values (assert)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (obj).</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>toBeDefined</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(expectationFailOutput)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (obj).</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>toBeNull</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(expectationFailOutput)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(obj).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6F42C1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>toBeNull</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(expectationFailOutput);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(obj).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6F42C1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>toEqual</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(any, expectationFailOutput?);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(obj).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6F42C1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>toBeDefined</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(expectationFailOutput?);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(obj).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6F42C1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>toBeUndefined</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(expectationFailOutput?);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (obj).</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>toBe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(any, expectationFailOutput)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(obj).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6F42C1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>toBe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(any, expectationFailOutput?);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>suite of tests, what we're testing</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-&gt; describe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">( description, () =&gt;{ ... }) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>suite of tests/specs, what we are testing</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">result to expect -&gt;  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>expect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (obj).</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>toEqual</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(any)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1  test/spec-&gt;   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>it</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">( description, () =&gt;{ ... })                       
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Here we're testing everting under MasterController class</t>
+  </si>
+  <si>
+    <t>masterController.ts</t>
+  </si>
+  <si>
+    <t>masterControllerSpec.ts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1633,6 +1983,30 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF9933"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1708,7 +2082,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1772,6 +2146,18 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1781,9 +2167,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9933"/>
       <color rgb="FFFFCC99"/>
       <color rgb="FFFFCC00"/>
-      <color rgb="FFFF9933"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1799,15 +2185,90 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>206375</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>25318</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4460875</xdr:colOff>
-      <xdr:row>274</xdr:row>
-      <xdr:rowOff>142877</xdr:rowOff>
+      <xdr:colOff>4476749</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>173799</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="72" name="Group 71"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="0" y="14519193"/>
+          <a:ext cx="11350624" cy="19309606"/>
+          <a:chOff x="0" y="14519193"/>
+          <a:chExt cx="11350624" cy="19134981"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="5" name="Picture 4"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="0" y="14519193"/>
+            <a:ext cx="11331575" cy="4923333"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="71" name="Picture 70"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="0" y="19399249"/>
+            <a:ext cx="11350624" cy="14254925"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>658812</xdr:colOff>
+      <xdr:row>278</xdr:row>
+      <xdr:rowOff>134940</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -1816,8 +2277,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="206375" y="9485313"/>
-          <a:ext cx="11136313" cy="45450127"/>
+          <a:off x="35528249" y="10326688"/>
+          <a:ext cx="11136313" cy="45751752"/>
           <a:chOff x="15875" y="4318000"/>
           <a:chExt cx="6210980" cy="27082750"/>
         </a:xfrm>
@@ -1830,7 +2291,7 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
           <a:stretch>
             <a:fillRect/>
           </a:stretch>
@@ -1853,7 +2314,7 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
           <a:stretch>
             <a:fillRect/>
           </a:stretch>
@@ -1876,7 +2337,7 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
           <a:stretch>
             <a:fillRect/>
           </a:stretch>
@@ -1915,7 +2376,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1953,7 +2414,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1962,6 +2423,1632 @@
         <a:xfrm>
           <a:off x="21002624" y="47625"/>
           <a:ext cx="5540375" cy="3161572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1451427</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>88901</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15068550" y="10801351"/>
+          <a:ext cx="8595177" cy="14116050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2686050</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4267200" y="15868650"/>
+          <a:ext cx="13487400" cy="76200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3429000</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1905000</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3429000" y="13693775"/>
+          <a:ext cx="14525625" cy="2101850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2647950</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4514850" y="15982950"/>
+          <a:ext cx="13201650" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1943100</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4152900" y="16021050"/>
+          <a:ext cx="17221200" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1571625</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2279650</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>44452</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1571625" y="15986125"/>
+          <a:ext cx="708025" cy="1917702"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1778000</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>174627</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2349500</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Arrow Connector 36"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1778000" y="16208377"/>
+          <a:ext cx="571500" cy="1539873"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2778126</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>158751</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3381375</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Straight Arrow Connector 41"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2778126" y="16811626"/>
+          <a:ext cx="603249" cy="1587499"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2381251</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2968625</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Arrow Connector 43"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2381251" y="16589376"/>
+          <a:ext cx="587374" cy="1682749"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2111376</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>177720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2667000</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Straight Arrow Connector 53"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2111376" y="16417845"/>
+          <a:ext cx="555624" cy="1727280"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1390652</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1936750</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="Straight Arrow Connector 58"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1390652" y="15836900"/>
+          <a:ext cx="546098" cy="3149600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2587625</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2571750</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="64" name="Elbow Connector 63"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2587625" y="18161000"/>
+          <a:ext cx="3937000" cy="809625"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -1613"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>492125</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2841625</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="74" name="Straight Arrow Connector 73"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4445000" y="16303625"/>
+          <a:ext cx="14446250" cy="3381375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>873125</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3667125</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>25319</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="76" name="Straight Arrow Connector 75"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4826000" y="13938250"/>
+          <a:ext cx="14890750" cy="6232444"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4079875</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>15878</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1095375</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="78" name="Straight Arrow Connector 77"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10953750" y="18827753"/>
+          <a:ext cx="6191250" cy="2127247"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1428749</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4206874</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="83" name="Right Brace 82"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8302624" y="20732750"/>
+          <a:ext cx="2778125" cy="1746250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 8333"/>
+            <a:gd name="adj2" fmla="val 12727"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1397000</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>31749</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4381500</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>79374</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="86" name="Right Brace 85"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8270875" y="22653624"/>
+          <a:ext cx="2984500" cy="1190625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 8333"/>
+            <a:gd name="adj2" fmla="val 54167"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4381500</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1158875</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>105175</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="87" name="Straight Arrow Connector 86"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="86" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11255375" y="19065875"/>
+          <a:ext cx="5953125" cy="4232675"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1174750</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="90" name="Right Brace 89"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8207375" y="23987125"/>
+          <a:ext cx="4333875" cy="3651250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1063625</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4635501</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>111126</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="91" name="Straight Arrow Connector 90"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="94" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12430125" y="21685250"/>
+          <a:ext cx="3571876" cy="4222751"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4635501</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1063626</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="94" name="Left Brace 93"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16002001" y="19415125"/>
+          <a:ext cx="1111250" cy="4413250"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1079500</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1809750</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="97" name="Straight Arrow Connector 96"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5032375" y="12398375"/>
+          <a:ext cx="12827000" cy="9223375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1222375</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1809750</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="98" name="Straight Arrow Connector 97"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5175250" y="12731750"/>
+          <a:ext cx="12684125" cy="9318626"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3619500</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>682625</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="103" name="Elbow Connector 102"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3619500" y="13700125"/>
+          <a:ext cx="13938250" cy="5857875"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>555625</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>351265</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="108" name="Picture 107"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24558625" y="27701875"/>
+          <a:ext cx="7653765" cy="5794375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>31749</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2968625</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="110" name="Curved Connector 109"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="3968750" y="17700624"/>
+          <a:ext cx="15875000" cy="11795125"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 1800"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2746375</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="113" name="Curved Connector 112"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4175125" y="17097375"/>
+          <a:ext cx="15446375" cy="11287125"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 91932"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2524124</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>365325</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="115" name="Picture 114"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13890624" y="27670125"/>
+          <a:ext cx="10477701" cy="4349750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>587376</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>79374</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3889376</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>57067</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="116" name="Curved Connector 115"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3281404" y="13355596"/>
+          <a:ext cx="18741943" cy="16224250"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 112765"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2682875</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2079625</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="122" name="Straight Arrow Connector 121"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2682875" y="31289625"/>
+          <a:ext cx="3349625" cy="587375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3921125</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1793875</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="124" name="Straight Arrow Connector 123"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3921125" y="32067500"/>
+          <a:ext cx="1825625" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3873500</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2492375</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="126" name="Straight Arrow Connector 125"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3873500" y="32353250"/>
+          <a:ext cx="2571750" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1111250</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2619375</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="131" name="Straight Arrow Connector 130"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5064125" y="31940500"/>
+          <a:ext cx="1508125" cy="1127125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>555625</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4429125</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>103178</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="133" name="Picture 132"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="555625" y="34004250"/>
+          <a:ext cx="10747375" cy="7373928"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2260,10 +4347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G158"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F180" sqref="F180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2271,7 +4358,7 @@
     <col min="1" max="1" width="59.28515625" customWidth="1"/>
     <col min="2" max="2" width="43.85546875" customWidth="1"/>
     <col min="3" max="3" width="67.42578125" customWidth="1"/>
-    <col min="4" max="4" width="55.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="82.7109375" style="7" customWidth="1"/>
     <col min="5" max="5" width="65.28515625" style="8" customWidth="1"/>
     <col min="6" max="6" width="41.5703125" customWidth="1"/>
   </cols>
@@ -2281,7 +4368,7 @@
         <v>0</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G1" s="8"/>
     </row>
@@ -2299,22 +4386,22 @@
     </row>
     <row r="3" spans="1:7" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -2324,7 +4411,7 @@
     </row>
     <row r="5" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="8"/>
@@ -2335,7 +4422,7 @@
     </row>
     <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="11"/>
       <c r="F7" s="7"/>
@@ -2343,10 +4430,10 @@
     </row>
     <row r="8" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="C8" s="4"/>
       <c r="F8" s="7"/>
@@ -2354,230 +4441,341 @@
     </row>
     <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>40</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="E24" s="26"/>
     </row>
     <row r="25" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C25" s="19" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="C26" s="13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C27" s="7"/>
       <c r="D27" s="14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C28" s="7"/>
       <c r="D28" s="14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C29" s="7"/>
       <c r="D29" s="14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C30" s="7"/>
       <c r="D30" s="14" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E43" s="28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D63" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D69" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D70" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="4:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D71" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D72" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="4:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D73" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="4:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D74" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76" spans="4:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D76" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="4:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D77" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="4:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D78" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D79" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D80" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D86" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="88" spans="4:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D88" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D89" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D90" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="91" spans="4:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D91" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D101" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D102" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="158" spans="4:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D158" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>